<commit_message>
Data and Code Updates
Fixing of data, figures, and code.
</commit_message>
<xml_diff>
--- a/Tables and Figures/Stats Tables.xlsx
+++ b/Tables and Figures/Stats Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\PhD\magnet.hypothesis.Mojave\Tables and Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33228D9D-AA8D-4750-BC89-C94852B383DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307CA931-FD8F-43C0-A8AA-2BAD5FA81EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85FA6EDC-8679-4757-82C0-CCAE0B1842B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>Larrea - open</t>
   </si>
@@ -60,9 +60,6 @@
     <t>&lt;0.0001*</t>
   </si>
   <si>
-    <t>0.040*</t>
-  </si>
-  <si>
     <t>bees - flies</t>
   </si>
   <si>
@@ -81,49 +78,13 @@
     <t>0.0003*</t>
   </si>
   <si>
-    <t>2.78 (0.305)</t>
-  </si>
-  <si>
-    <t>1.76 (0.327)</t>
-  </si>
-  <si>
-    <t>1.18 (0.557)</t>
-  </si>
-  <si>
-    <t>0.035*</t>
-  </si>
-  <si>
     <t>1.61 (0.693)</t>
   </si>
   <si>
-    <t>0.892 (0.264)</t>
-  </si>
-  <si>
-    <t>0.0023*</t>
-  </si>
-  <si>
-    <t>2.28 (0.468)</t>
-  </si>
-  <si>
-    <t>1.39 (0.499)</t>
-  </si>
-  <si>
-    <t>0.016*</t>
-  </si>
-  <si>
-    <t>1.36 (0.589)</t>
-  </si>
-  <si>
-    <t>0.022*</t>
-  </si>
-  <si>
     <t>Insect RTU</t>
   </si>
   <si>
     <t>Shrub Volume</t>
-  </si>
-  <si>
-    <t>0.0041*</t>
   </si>
   <si>
     <r>
@@ -290,42 +251,15 @@
     <t>without annuals</t>
   </si>
   <si>
-    <t>1.93 (0.36)</t>
-  </si>
-  <si>
     <t>log estimate (SE)</t>
   </si>
   <si>
-    <t>2.10 (0.289)</t>
-  </si>
-  <si>
-    <t>3.71 (0.644)</t>
-  </si>
-  <si>
-    <t>0.026*</t>
-  </si>
-  <si>
-    <t>-1.30 (1.06)</t>
-  </si>
-  <si>
-    <t>1.17 (0.54)</t>
-  </si>
-  <si>
-    <t>2.69 (0.47)</t>
-  </si>
-  <si>
-    <t>0.005*</t>
-  </si>
-  <si>
     <t>Ambrosia</t>
   </si>
   <si>
     <t>4.44 (0.493)</t>
   </si>
   <si>
-    <t>1.74 (0.557)</t>
-  </si>
-  <si>
     <t>2.33 (0.321)</t>
   </si>
   <si>
@@ -335,70 +269,13 @@
     <t>0.0017*</t>
   </si>
   <si>
-    <t>2.18 (0.184)</t>
-  </si>
-  <si>
-    <t>4.16 (0.270)</t>
-  </si>
-  <si>
     <t>1.98 (0.296)</t>
   </si>
   <si>
-    <t>-0.106 (0.229)</t>
-  </si>
-  <si>
-    <t>-0.206 (0.302)</t>
-  </si>
-  <si>
-    <t>-0.100 (0.323)</t>
-  </si>
-  <si>
-    <t>-0.475 (0.417)</t>
-  </si>
-  <si>
     <t>-1.38 (0.437)</t>
   </si>
   <si>
-    <t>-0.906 (0.432)</t>
-  </si>
-  <si>
-    <t>-0.442 (0.629)</t>
-  </si>
-  <si>
-    <t>-0.703 (0.639)</t>
-  </si>
-  <si>
-    <t>-0.262 (0.622)</t>
-  </si>
-  <si>
     <t>2.70 (0.349)</t>
-  </si>
-  <si>
-    <t>4.10 (0.454)</t>
-  </si>
-  <si>
-    <t>1.77 (0.509)</t>
-  </si>
-  <si>
-    <t>1.52 (0.282)</t>
-  </si>
-  <si>
-    <t>3.94 (0.447)</t>
-  </si>
-  <si>
-    <t>2.42 (0.475)</t>
-  </si>
-  <si>
-    <t>0.033*</t>
-  </si>
-  <si>
-    <t>-2.05 (0.911)</t>
-  </si>
-  <si>
-    <t>-2.81 (0.892)</t>
-  </si>
-  <si>
-    <t>0.0022*</t>
   </si>
   <si>
     <r>
@@ -731,6 +608,126 @@
       </rPr>
       <t xml:space="preserve"> without annuals</t>
     </r>
+  </si>
+  <si>
+    <t>0.888 (0.265)</t>
+  </si>
+  <si>
+    <t>0.0029*</t>
+  </si>
+  <si>
+    <t>2.27 (0.469)</t>
+  </si>
+  <si>
+    <t>1.38 (0.500)</t>
+  </si>
+  <si>
+    <t>0.018*</t>
+  </si>
+  <si>
+    <t>1.38 (0.575)</t>
+  </si>
+  <si>
+    <t>0.036*</t>
+  </si>
+  <si>
+    <t>0.048*</t>
+  </si>
+  <si>
+    <t>2.75 (0.304)</t>
+  </si>
+  <si>
+    <t>1.73 (0.325)</t>
+  </si>
+  <si>
+    <t>1.19 (0.557)</t>
+  </si>
+  <si>
+    <t>0.034*</t>
+  </si>
+  <si>
+    <t>2.11 (0.289)</t>
+  </si>
+  <si>
+    <t>3.72 (0.644)</t>
+  </si>
+  <si>
+    <t>2.19 (0.184)</t>
+  </si>
+  <si>
+    <t>4.16 (0.269)</t>
+  </si>
+  <si>
+    <t>-0.105 (0.228)</t>
+  </si>
+  <si>
+    <t>-0.210 (0.302)</t>
+  </si>
+  <si>
+    <t>-0.105 (0.323)</t>
+  </si>
+  <si>
+    <t>-0.474 (0.417)</t>
+  </si>
+  <si>
+    <t>0.0049*</t>
+  </si>
+  <si>
+    <t>-0.910 (0.432)</t>
+  </si>
+  <si>
+    <t>-0.443 (0.629)</t>
+  </si>
+  <si>
+    <t>-0.704 (0.640)</t>
+  </si>
+  <si>
+    <t>-0.261 (0.622)</t>
+  </si>
+  <si>
+    <t>1.74 (0.556)</t>
+  </si>
+  <si>
+    <t>4.10 (0.453)</t>
+  </si>
+  <si>
+    <t>1.77 (0.508)</t>
+  </si>
+  <si>
+    <t>2.42 (0.474)</t>
+  </si>
+  <si>
+    <t>3.95 (0.447)</t>
+  </si>
+  <si>
+    <t>1.53 (0.282)</t>
+  </si>
+  <si>
+    <t>-2.15 (0.900)</t>
+  </si>
+  <si>
+    <t>0.019*</t>
+  </si>
+  <si>
+    <t>1.95 (0.361)</t>
+  </si>
+  <si>
+    <t>-2.90 (0.88)</t>
+  </si>
+  <si>
+    <t>0.0014*</t>
+  </si>
+  <si>
+    <t>-1.40 (1.05)</t>
+  </si>
+  <si>
+    <t>1.20 (0.538)</t>
+  </si>
+  <si>
+    <t>0.028*</t>
+  </si>
+  <si>
+    <t>2.70 (0.469)</t>
   </si>
 </sst>
 </file>
@@ -1337,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D81387-9119-42C1-8255-2CFCA08B4879}">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1372,13 +1369,13 @@
       <c r="J1" s="46"/>
       <c r="K1" s="22"/>
       <c r="L1" s="23" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O1" s="23" t="s">
         <v>5</v>
@@ -1390,7 +1387,7 @@
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>4</v>
@@ -1399,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>4</v>
@@ -1408,7 +1405,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
@@ -1417,7 +1414,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1435,10 +1432,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B4" s="11">
-        <v>8.6300000000000008</v>
+        <v>8.65</v>
       </c>
       <c r="C4" s="11">
         <v>1</v>
@@ -1447,34 +1444,34 @@
         <v>6</v>
       </c>
       <c r="E4" s="11">
-        <v>4.2300000000000004</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="F4" s="11">
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="K4" s="28"/>
       <c r="L4" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="N4" s="30">
-        <v>2.38</v>
+        <v>3.35</v>
       </c>
       <c r="O4" s="30" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B5" s="11">
-        <v>30.1</v>
+        <v>30</v>
       </c>
       <c r="C5" s="11">
         <v>2</v>
@@ -1483,7 +1480,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="11">
-        <v>84.2</v>
+        <v>83.1</v>
       </c>
       <c r="F5" s="11">
         <v>2</v>
@@ -1493,13 +1490,13 @@
       </c>
       <c r="K5" s="28"/>
       <c r="L5" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="N5" s="30">
-        <v>4.87</v>
+        <v>4.83</v>
       </c>
       <c r="O5" s="30" t="s">
         <v>7</v>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B6" s="11">
         <v>15.2</v>
@@ -1522,26 +1519,26 @@
         <v>7</v>
       </c>
       <c r="E6" s="11">
-        <v>3.71</v>
+        <v>3.92</v>
       </c>
       <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6" s="11">
-        <v>5.3999999999999999E-2</v>
+      <c r="G6" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="N6" s="30">
-        <v>2.78</v>
+        <v>2.76</v>
       </c>
       <c r="O6" s="30" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" s="21"/>
@@ -1549,38 +1546,38 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B7" s="15">
-        <v>0.61</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="C7" s="11">
         <v>2</v>
       </c>
       <c r="D7" s="11">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="E7" s="11">
-        <v>3.53</v>
+        <v>3.38</v>
       </c>
       <c r="F7" s="11">
         <v>2</v>
       </c>
       <c r="G7" s="11">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="K7" s="28"/>
       <c r="L7" s="27" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="N7" s="30">
-        <v>2.31</v>
+        <v>2.39</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="21"/>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="5"/>
@@ -1617,13 +1614,13 @@
       <c r="G9" s="5"/>
       <c r="K9" s="28"/>
       <c r="L9" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="N9" s="30">
-        <v>7.28</v>
+        <v>7.3</v>
       </c>
       <c r="O9" s="30" t="s">
         <v>7</v>
@@ -1631,19 +1628,19 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B10" s="11">
-        <v>2.4</v>
+        <v>2.15</v>
       </c>
       <c r="C10" s="11">
         <v>2</v>
       </c>
       <c r="D10" s="11">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="E10" s="11">
-        <v>4.2300000000000004</v>
+        <v>4.26</v>
       </c>
       <c r="F10" s="11">
         <v>2</v>
@@ -1653,13 +1650,13 @@
       </c>
       <c r="K10" s="28"/>
       <c r="L10" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="N10" s="30">
-        <v>5.77</v>
+        <v>5.78</v>
       </c>
       <c r="O10" s="30" t="s">
         <v>7</v>
@@ -1667,10 +1664,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11">
-        <v>84.2</v>
+        <v>84.8</v>
       </c>
       <c r="C11" s="11">
         <v>2</v>
@@ -1679,7 +1676,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="11">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F11" s="11">
         <v>2</v>
@@ -1689,10 +1686,10 @@
       </c>
       <c r="K11" s="28"/>
       <c r="L11" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N11" s="30">
         <v>2.33</v>
@@ -1703,25 +1700,25 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11">
-        <v>1.96</v>
+        <v>1.67</v>
       </c>
       <c r="C12" s="11">
         <v>1</v>
       </c>
       <c r="D12" s="11">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="11">
-        <v>0.24399999999999999</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="F12" s="11">
         <v>1</v>
       </c>
       <c r="G12" s="11">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="27"/>
@@ -1731,10 +1728,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B13" s="11">
-        <v>0.69299999999999995</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="C13" s="11">
         <v>4</v>
@@ -1752,7 +1749,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
@@ -1777,7 +1774,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="5"/>
@@ -1787,49 +1784,49 @@
       <c r="G15" s="5"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M15" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="30">
+        <v>4.01</v>
+      </c>
+      <c r="O15" s="30" t="s">
         <v>13</v>
-      </c>
-      <c r="N15" s="30">
-        <v>4</v>
-      </c>
-      <c r="O15" s="30" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B16" s="11">
-        <v>2.0199999999999999E-2</v>
+        <v>2.1299999999999999E-2</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
       </c>
       <c r="D16" s="11">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="E16" s="11">
-        <v>8.26</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M16" s="29" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="N16" s="30">
-        <v>9.1300000000000008</v>
+        <v>9.06</v>
       </c>
       <c r="O16" s="30" t="s">
         <v>7</v>
@@ -1837,10 +1834,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B17" s="11">
-        <v>0.38900000000000001</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="C17" s="11">
         <v>2</v>
@@ -1849,7 +1846,7 @@
         <v>0.53</v>
       </c>
       <c r="E17" s="11">
-        <v>32.299999999999997</v>
+        <v>32.9</v>
       </c>
       <c r="F17" s="11">
         <v>2</v>
@@ -1859,13 +1856,13 @@
       </c>
       <c r="K17" s="27"/>
       <c r="L17" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="N17" s="30">
-        <v>5.4</v>
+        <v>5.32</v>
       </c>
       <c r="O17" s="30" t="s">
         <v>7</v>
@@ -1873,16 +1870,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B18" s="11">
-        <v>1.3599999999999999E-2</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
       </c>
       <c r="D18" s="11">
-        <v>0.91</v>
+        <v>0.94</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1892,21 +1889,21 @@
         <v>0</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="N18" s="30">
-        <v>2.12</v>
+        <v>2.14</v>
       </c>
       <c r="O18" s="30" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B19" s="11">
-        <v>4.7000000000000002E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -1915,13 +1912,13 @@
         <v>0.95</v>
       </c>
       <c r="E19" s="11">
-        <v>2.63</v>
+        <v>2.97</v>
       </c>
       <c r="F19" s="11">
         <v>1</v>
       </c>
-      <c r="G19" s="16">
-        <v>0.1</v>
+      <c r="G19" s="15">
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="K19" s="31">
         <v>2016</v>
@@ -1933,32 +1930,32 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B20" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>1.21E-2</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
       </c>
       <c r="D20" s="11">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="E20" s="11">
-        <v>0.70499999999999996</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="F20" s="11">
         <v>1</v>
       </c>
       <c r="G20" s="16">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="N20" s="30">
         <v>11.9</v>
@@ -1969,10 +1966,10 @@
     </row>
     <row r="21" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B21" s="13">
-        <v>2.7000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="C21" s="13">
         <v>2</v>
@@ -1981,23 +1978,23 @@
         <v>0.96</v>
       </c>
       <c r="E21" s="13">
-        <v>4.57</v>
+        <v>4.49</v>
       </c>
       <c r="F21" s="13">
         <v>2</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="N21" s="30">
-        <v>15.4</v>
+        <v>15.5</v>
       </c>
       <c r="O21" s="30" t="s">
         <v>7</v>
@@ -2007,13 +2004,13 @@
       <c r="A22" s="18"/>
       <c r="K22" s="27"/>
       <c r="L22" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="N22" s="30">
-        <v>6.66</v>
+        <v>6.67</v>
       </c>
       <c r="O22" s="30" t="s">
         <v>7</v>
@@ -2022,16 +2019,16 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="K23" s="27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="L23" s="32" t="s">
         <v>1</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="N23" s="30">
-        <v>-0.46400000000000002</v>
+        <v>-0.46100000000000002</v>
       </c>
       <c r="O23" s="33">
         <v>0.89129999999999998</v>
@@ -2041,13 +2038,13 @@
       <c r="A24" s="19"/>
       <c r="K24" s="27"/>
       <c r="L24" s="27" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="M24" s="29" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="N24" s="30">
-        <v>-0.68200000000000005</v>
+        <v>-0.69599999999999995</v>
       </c>
       <c r="O24" s="33">
         <v>0.77</v>
@@ -2057,28 +2054,28 @@
       <c r="A25" s="19"/>
       <c r="K25" s="27"/>
       <c r="L25" s="27" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="N25" s="34">
-        <v>-0.31</v>
+        <v>-0.32600000000000001</v>
       </c>
       <c r="O25" s="33">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="K26" s="27" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L26" s="32" t="s">
         <v>1</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="N26" s="33">
         <v>-1.1399999999999999</v>
@@ -2091,47 +2088,47 @@
       <c r="A27" s="19"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="N27" s="33">
-        <v>-3.16</v>
+        <v>-3.17</v>
       </c>
       <c r="O27" s="34" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="K28" s="27"/>
       <c r="L28" s="27" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="M28" s="29" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="N28" s="33">
-        <v>-2.1</v>
+        <v>-2.11</v>
       </c>
       <c r="O28" s="34">
-        <v>9.1999999999999998E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="K29" s="27" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="L29" s="32" t="s">
         <v>1</v>
       </c>
       <c r="M29" s="29" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="N29" s="34">
-        <v>-0.70199999999999996</v>
+        <v>-0.70399999999999996</v>
       </c>
       <c r="O29" s="33">
         <v>0.76</v>
@@ -2141,26 +2138,26 @@
       <c r="A30" s="19"/>
       <c r="K30" s="27"/>
       <c r="L30" s="27" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="M30" s="29" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="N30" s="33">
         <v>-1.1000000000000001</v>
       </c>
       <c r="O30" s="33">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="K31" s="27"/>
       <c r="L31" s="27" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="M31" s="29" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="N31" s="34">
         <v>-0.42</v>
@@ -2172,16 +2169,16 @@
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="K32" s="32" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="L32" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M32" s="30" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="N32" s="33">
-        <v>7.74</v>
+        <v>7.75</v>
       </c>
       <c r="O32" s="30" t="s">
         <v>7</v>
@@ -2191,13 +2188,13 @@
       <c r="A33" s="19"/>
       <c r="K33" s="27"/>
       <c r="L33" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M33" s="30" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="N33" s="33">
-        <v>9.01</v>
+        <v>9.02</v>
       </c>
       <c r="O33" s="30" t="s">
         <v>7</v>
@@ -2207,31 +2204,31 @@
       <c r="A34" s="19"/>
       <c r="K34" s="27"/>
       <c r="L34" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M34" s="30" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="N34" s="33">
         <v>3.1259999999999999</v>
       </c>
       <c r="O34" s="30" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="K35" s="32" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="L35" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M35" s="30" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="N35" s="33">
-        <v>7.26</v>
+        <v>7.27</v>
       </c>
       <c r="O35" s="30" t="s">
         <v>7</v>
@@ -2241,13 +2238,13 @@
       <c r="A36" s="2"/>
       <c r="K36" s="27"/>
       <c r="L36" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M36" s="30" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="N36" s="33">
-        <v>9.0419999999999998</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="O36" s="30" t="s">
         <v>7</v>
@@ -2257,31 +2254,31 @@
       <c r="A37" s="2"/>
       <c r="K37" s="27"/>
       <c r="L37" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M37" s="30" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="N37" s="33">
         <v>3.48</v>
       </c>
       <c r="O37" s="30" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="K38" s="27" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="L38" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M38" s="30" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="N38" s="33">
-        <v>5.4</v>
+        <v>5.42</v>
       </c>
       <c r="O38" s="30" t="s">
         <v>7</v>
@@ -2290,13 +2287,13 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K39" s="27"/>
       <c r="L39" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M39" s="30" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="N39" s="33">
-        <v>8.82</v>
+        <v>8.84</v>
       </c>
       <c r="O39" s="30" t="s">
         <v>7</v>
@@ -2305,13 +2302,13 @@
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K40" s="27"/>
       <c r="L40" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M40" s="30" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="N40" s="33">
-        <v>5.09</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="O40" s="30" t="s">
         <v>7</v>
@@ -2326,7 +2323,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K42" s="35" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="L42" s="27"/>
       <c r="M42" s="27"/>
@@ -2336,13 +2333,13 @@
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K43" s="27"/>
       <c r="L43" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M43" s="30" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="N43" s="30">
-        <v>5.33</v>
+        <v>5.4</v>
       </c>
       <c r="O43" s="30" t="s">
         <v>7</v>
@@ -2351,47 +2348,47 @@
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K44" s="27"/>
       <c r="L44" s="31" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="M44" s="36" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="N44" s="30">
-        <v>-2.5499999999999998</v>
+        <v>-2.39</v>
       </c>
       <c r="O44" s="30" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K45" s="27" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="L45" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M45" s="30" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="N45" s="30">
-        <v>2.17</v>
+        <v>2.23</v>
       </c>
       <c r="O45" s="30" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K46" s="27" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="L46" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M46" s="30" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="N46" s="30">
-        <v>5.71</v>
+        <v>5.75</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>7</v>
@@ -2399,36 +2396,36 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K47" s="27" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="L47" s="31" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="M47" s="29" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="N47" s="30">
-        <v>-3.15</v>
+        <v>-3.29</v>
       </c>
       <c r="O47" s="30" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K48" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="M48" s="37" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="N48" s="4">
-        <v>-1.23</v>
+        <v>-1.34</v>
       </c>
       <c r="O48" s="4">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -2464,7 +2461,7 @@
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="38" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>4</v>
@@ -2477,13 +2474,13 @@
       <c r="G1" s="1"/>
       <c r="H1" s="40"/>
       <c r="I1" s="41" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="J1" s="39" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>5</v>
@@ -2491,7 +2488,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -2501,7 +2498,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="42"/>
       <c r="I2" s="43" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="30"/>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B3" s="27">
         <v>327</v>
@@ -2525,10 +2522,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="42"/>
       <c r="I3" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="K3" s="30">
         <v>1.78</v>
@@ -2539,7 +2536,7 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B4" s="27">
         <v>4.24</v>
@@ -2555,10 +2552,10 @@
       <c r="G4" s="1"/>
       <c r="H4" s="42"/>
       <c r="I4" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="K4" s="30">
         <v>-9.1199999999999992</v>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B5" s="27">
         <v>67.2</v>
@@ -2585,10 +2582,10 @@
       <c r="G5" s="1"/>
       <c r="H5" s="42"/>
       <c r="I5" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="K5" s="30">
         <v>-18.5</v>
@@ -2609,10 +2606,10 @@
         <v>2015</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="K6" s="30">
         <v>-6.38</v>
@@ -2633,10 +2630,10 @@
       <c r="G7" s="1"/>
       <c r="H7" s="42"/>
       <c r="I7" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="K7" s="30">
         <v>0.51100000000000001</v>
@@ -2647,7 +2644,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B8" s="27">
         <v>165</v>
@@ -2665,10 +2662,10 @@
         <v>2016</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="K8" s="30">
         <v>-4.76</v>
@@ -2687,10 +2684,10 @@
       <c r="G9" s="1"/>
       <c r="H9" s="42"/>
       <c r="I9" s="44" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="K9" s="30">
         <v>0.53200000000000003</v>
@@ -2701,7 +2698,7 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -2711,21 +2708,21 @@
       <c r="G10" s="1"/>
       <c r="H10" s="42"/>
       <c r="I10" s="44" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="K10" s="30">
         <v>-4.2300000000000004</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B11" s="27">
         <v>102</v>
@@ -2741,10 +2738,10 @@
       <c r="G11" s="1"/>
       <c r="H11" s="42"/>
       <c r="I11" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="K11" s="30">
         <v>7.8</v>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B12" s="27">
         <v>7.97</v>
@@ -2764,19 +2761,19 @@
         <v>1</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="42" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="K12" s="30">
         <v>0.76600000000000001</v>
@@ -2787,7 +2784,7 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B13" s="27">
         <v>15.9</v>
@@ -2796,19 +2793,19 @@
         <v>2</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="44" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="K13" s="30">
         <v>8.2000000000000003E-2</v>
@@ -2826,13 +2823,13 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="42" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="K14" s="30">
         <v>4.25</v>
@@ -2859,7 +2856,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3">
         <v>39.5</v>
@@ -2875,7 +2872,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="42"/>
       <c r="I16" s="43" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
@@ -2891,16 +2888,16 @@
       <c r="G17" s="1"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="K17" s="30">
         <v>-3.31</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2913,10 +2910,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="42"/>
       <c r="I18" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J18" s="29" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="K18" s="30">
         <v>-5.12</v>
@@ -2935,16 +2932,16 @@
       <c r="G19" s="1"/>
       <c r="H19" s="42"/>
       <c r="I19" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="K19" s="30">
         <v>3.29</v>
       </c>
       <c r="L19" s="30" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2959,10 +2956,10 @@
         <v>2015</v>
       </c>
       <c r="I20" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="K20" s="30">
         <v>-2.23</v>
@@ -2981,10 +2978,10 @@
       <c r="G21" s="1"/>
       <c r="H21" s="42"/>
       <c r="I21" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="K21" s="30">
         <v>0.64600000000000002</v>
@@ -3005,16 +3002,16 @@
         <v>2016</v>
       </c>
       <c r="I22" s="44" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="K22" s="30">
         <v>-3.56</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3027,10 +3024,10 @@
       <c r="G23" s="1"/>
       <c r="H23" s="42"/>
       <c r="I23" s="44" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="K23" s="30">
         <v>0.25900000000000001</v>
@@ -3049,16 +3046,16 @@
       <c r="G24" s="1"/>
       <c r="H24" s="42"/>
       <c r="I24" s="44" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="K24" s="30">
         <v>-3.3</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3071,16 +3068,16 @@
       <c r="G25" s="1"/>
       <c r="H25" s="42"/>
       <c r="I25" s="44" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="K25" s="30">
         <v>2.7</v>
       </c>
       <c r="L25" s="30" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3092,13 +3089,13 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="42" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="K26" s="30">
         <v>-4.25</v>
@@ -3116,19 +3113,19 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="44" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="I27" s="42" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="K27" s="30">
         <v>-2.5</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3140,13 +3137,13 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="45" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="I28" s="45" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="K28" s="4">
         <v>0.104</v>

</xml_diff>

<commit_message>
Figure and Table Edits
Figure and Table edits for publication.
</commit_message>
<xml_diff>
--- a/Tables and Figures/Stats Tables.xlsx
+++ b/Tables and Figures/Stats Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\PhD\magnet.hypothesis.Mojave\Tables and Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307CA931-FD8F-43C0-A8AA-2BAD5FA81EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187570A6-BB75-4D38-9401-5A54D8F401ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85FA6EDC-8679-4757-82C0-CCAE0B1842B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="133">
   <si>
     <t>Larrea - open</t>
   </si>
@@ -703,31 +703,34 @@
     <t>1.53 (0.282)</t>
   </si>
   <si>
-    <t>-2.15 (0.900)</t>
-  </si>
-  <si>
-    <t>0.019*</t>
-  </si>
-  <si>
-    <t>1.95 (0.361)</t>
-  </si>
-  <si>
-    <t>-2.90 (0.88)</t>
-  </si>
-  <si>
-    <t>0.0014*</t>
-  </si>
-  <si>
-    <t>-1.40 (1.05)</t>
-  </si>
-  <si>
-    <t>1.20 (0.538)</t>
-  </si>
-  <si>
-    <t>0.028*</t>
-  </si>
-  <si>
-    <t>2.70 (0.469)</t>
+    <t>0.0016*</t>
+  </si>
+  <si>
+    <t>0.032*</t>
+  </si>
+  <si>
+    <t>-2.84 (1.10)</t>
+  </si>
+  <si>
+    <t>0.012*</t>
+  </si>
+  <si>
+    <t>1.88 (0.353)</t>
+  </si>
+  <si>
+    <t>-3.58 (1.08)</t>
+  </si>
+  <si>
+    <t>0.0013*</t>
+  </si>
+  <si>
+    <t>-2.09 (1.23)</t>
+  </si>
+  <si>
+    <t>1.14 (0.521)</t>
+  </si>
+  <si>
+    <t>2.63 (0.467)</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D81387-9119-42C1-8255-2CFCA08B4879}">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1801,22 +1804,22 @@
         <v>21</v>
       </c>
       <c r="B16" s="11">
-        <v>2.1299999999999999E-2</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
       </c>
       <c r="D16" s="11">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="E16" s="11">
-        <v>9.1300000000000008</v>
+        <v>9.93</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="27" t="s">
@@ -1837,7 +1840,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="11">
-        <v>0.39300000000000002</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C17" s="11">
         <v>2</v>
@@ -1846,7 +1849,7 @@
         <v>0.53</v>
       </c>
       <c r="E17" s="11">
-        <v>32.9</v>
+        <v>31.4</v>
       </c>
       <c r="F17" s="11">
         <v>2</v>
@@ -1873,13 +1876,13 @@
         <v>22</v>
       </c>
       <c r="B18" s="11">
-        <v>6.4000000000000003E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
       </c>
       <c r="D18" s="11">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1903,22 +1906,22 @@
         <v>19</v>
       </c>
       <c r="B19" s="11">
-        <v>3.5999999999999999E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
       </c>
       <c r="D19" s="11">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="E19" s="11">
-        <v>2.97</v>
+        <v>3.67</v>
       </c>
       <c r="F19" s="11">
         <v>1</v>
       </c>
       <c r="G19" s="15">
-        <v>8.4000000000000005E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="K19" s="31">
         <v>2016</v>
@@ -1933,22 +1936,22 @@
         <v>16</v>
       </c>
       <c r="B20" s="11">
-        <v>1.21E-2</v>
+        <v>4.3E-3</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
       </c>
       <c r="D20" s="11">
-        <v>0.91</v>
+        <v>0.95</v>
       </c>
       <c r="E20" s="11">
-        <v>0.80600000000000005</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="F20" s="11">
         <v>1</v>
       </c>
       <c r="G20" s="16">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27" t="s">
@@ -1969,7 +1972,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="13">
-        <v>2.5000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="C21" s="13">
         <v>2</v>
@@ -1978,13 +1981,13 @@
         <v>0.96</v>
       </c>
       <c r="E21" s="13">
-        <v>4.49</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="F21" s="13">
         <v>2</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27" t="s">
@@ -2336,10 +2339,10 @@
         <v>8</v>
       </c>
       <c r="M43" s="30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N43" s="30">
-        <v>5.4</v>
+        <v>5.34</v>
       </c>
       <c r="O43" s="30" t="s">
         <v>7</v>
@@ -2351,13 +2354,13 @@
         <v>33</v>
       </c>
       <c r="M44" s="36" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N44" s="30">
-        <v>-2.39</v>
+        <v>-2.58</v>
       </c>
       <c r="O44" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2368,13 +2371,13 @@
         <v>8</v>
       </c>
       <c r="M45" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="N45" s="30">
-        <v>2.23</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="O45" s="30" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -2385,10 +2388,10 @@
         <v>8</v>
       </c>
       <c r="M46" s="30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N46" s="30">
-        <v>5.75</v>
+        <v>5.63</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>7</v>
@@ -2402,13 +2405,13 @@
         <v>33</v>
       </c>
       <c r="M47" s="29" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="N47" s="30">
-        <v>-3.29</v>
+        <v>-3.33</v>
       </c>
       <c r="O47" s="30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -2419,13 +2422,13 @@
         <v>33</v>
       </c>
       <c r="M48" s="37" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N48" s="4">
-        <v>-1.34</v>
+        <v>-1.7</v>
       </c>
       <c r="O48" s="4">
-        <v>0.18</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>